<commit_message>
[Nexial Expression] - [TEXT &raquo; `base64decodeThenSave(file,append)`] or [TEXT &raquo; `base64decode-then-save(file,append)`]: **NEW**   operation to perform BASE64 decoding on current TEXT content and then saving the decoded content to `file`. This is   useful when the decoded content is expected to be binary data.
Signed-off-by: automike <mikeliucc@users.noreply.github.com>
</commit_message>
<xml_diff>
--- a/src/test/resources/unittesting/artifact/data/unitTest_base_part3.data.xlsx
+++ b/src/test/resources/unittesting/artifact/data/unitTest_base_part3.data.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="10502"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="10512"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/ml093043/projects/nexial/nexial-core/src/test/resources/unittesting/artifact/data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C6F7257A-AAC5-F54C-8BDF-46A5F10C4AA5}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7B34D6DB-98DE-5E44-BBA6-9B6EEEE846E7}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="440" windowWidth="40960" windowHeight="8380" tabRatio="500" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="440" windowWidth="51200" windowHeight="10520" tabRatio="500" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="#default" sheetId="2" r:id="rId1"/>
@@ -37,10 +37,16 @@
     <definedName name="webcookie">'[1]#system'!$O$2:$O$8</definedName>
     <definedName name="ws">'[1]#system'!$P$2:$P$15</definedName>
   </definedNames>
-  <calcPr calcId="171027"/>
+  <calcPr calcId="191029"/>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{79F54976-1DA5-4618-B147-4CDE4B953A38}">
       <x14:workbookPr defaultImageDpi="32767"/>
+    </ext>
+    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
+      <xcalcf:calcFeatures>
+        <xcalcf:feature name="microsoft.com:RD"/>
+        <xcalcf:feature name="microsoft.com:FV"/>
+      </xcalcf:calcFeatures>
     </ext>
     <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{7523E5D3-25F3-A5E0-1632-64F254C22452}">
       <mx:ArchID Flags="2"/>
@@ -50,7 +56,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="16" uniqueCount="14">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="26" uniqueCount="24">
   <si>
     <t>true</t>
   </si>
@@ -92,6 +98,52 @@
   </si>
   <si>
     <t>Credits</t>
+  </si>
+  <si>
+    <t>text1.plain</t>
+  </si>
+  <si>
+    <t>Now is the time for all good men to come to the aid of the party</t>
+  </si>
+  <si>
+    <t>text2.plain</t>
+  </si>
+  <si>
+    <t>text3.plain</t>
+  </si>
+  <si>
+    <t>God grant me the serenity
+to accept the things I cannot change; 
+courage to change the things I can; 
+and wisdom to know the difference.
+Living one day at a time; 
+enjoying one moment at a time; 
+accepting hardships as the pathway to peace; 
+taking, as He did, this sinful world
+as it is, not as I would have it; 
+trusting that He will make all things right
+if I surrender to His Will; 
+that I may be reasonably happy in this life
+and supremely happy with Him
+forever in the next. 
+Amen.</t>
+  </si>
+  <si>
+    <t>Four score and seven years ago our fathers brought forth on this continent, a new nation, conceived in Liberty, and dedicated to the proposition that all men are created equal.
+Now we are engaged in a great civil war, testing whether that nation, or any nation so conceived and so dedicated, can long endure. We are met on a great battle-field of that war. We have come to dedicate a portion of that field, as a final resting place for those who here gave their lives that that nation might live. It is altogether fitting and proper that we should do this.
+But, in a larger sense, we can not dedicate -- we can not consecrate -- we can not hallow -- this ground. The brave men, living and dead, who struggled here, have consecrated it, far above our poor power to add or detract. The world will little note, nor long remember what we say here, but it can never forget what they did here. It is for us the living, rather, to be dedicated here to the unfinished work which they who fought here have thus far so nobly advanced. It is rather for us to be here dedicated to the great task remaining before us -- that from these honored dead we take increased devotion to that cause for which they gave the last full measure of devotion -- that we here highly resolve that these dead shall not have died in vain -- that this nation, under God, shall have a new birth of freedom -- and that government of the people, by the people, for the people, shall not perish from the earth.</t>
+  </si>
+  <si>
+    <t>text4.file</t>
+  </si>
+  <si>
+    <t>$(syspath|data|fullpath)/unitTest_base_part3.ico</t>
+  </si>
+  <si>
+    <t>text4.destination</t>
+  </si>
+  <si>
+    <t>$(syspath|out|fullpath)/decoded.ico</t>
   </si>
 </sst>
 </file>
@@ -186,7 +238,7 @@
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="7">
+  <cellXfs count="8">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="49" fontId="1" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="left" vertical="center"/>
@@ -208,6 +260,10 @@
     </xf>
     <xf numFmtId="49" fontId="3" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="left" vertical="center"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="49" fontId="2" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
       <protection locked="0"/>
     </xf>
   </cellXfs>
@@ -643,7 +699,7 @@
   <dimension ref="A1:AAA10"/>
   <sheetViews>
     <sheetView zoomScalePageLayoutView="125" workbookViewId="0">
-      <selection activeCell="A8" sqref="A8"/>
+      <selection activeCell="B9" sqref="B9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="17"/>
@@ -720,7 +776,7 @@
         <v>10</v>
       </c>
       <c r="B7" s="2" t="s">
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="HA7" s="4"/>
       <c r="AAA7" s="5"/>
@@ -767,14 +823,14 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{8B858EF3-1516-4B43-9DFB-8D7D7D41BDDA}">
   <dimension ref="A1:AAA10"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScalePageLayoutView="125" workbookViewId="0">
-      <selection activeCell="A2" sqref="A2"/>
+    <sheetView tabSelected="1" topLeftCell="A5" zoomScalePageLayoutView="125" workbookViewId="0">
+      <selection activeCell="A6" sqref="A6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="17"/>
   <cols>
     <col min="1" max="1" width="34" style="1" customWidth="1" collapsed="1"/>
-    <col min="2" max="2" width="27" style="2" customWidth="1" collapsed="1"/>
+    <col min="2" max="2" width="132.1640625" style="2" bestFit="1" customWidth="1" collapsed="1"/>
     <col min="3" max="9" width="27" style="3" customWidth="1" collapsed="1"/>
     <col min="10" max="27" width="21.1640625" style="3" customWidth="1" collapsed="1"/>
     <col min="28" max="16384" width="10.83203125" style="3" collapsed="1"/>
@@ -791,22 +847,52 @@
       <c r="AAA1" s="6"/>
     </row>
     <row r="2" spans="1:703">
+      <c r="A2" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="B2" s="2" t="s">
+        <v>15</v>
+      </c>
       <c r="HA2" s="6"/>
       <c r="AAA2" s="6"/>
     </row>
-    <row r="3" spans="1:703">
+    <row r="3" spans="1:703" ht="288">
+      <c r="A3" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="B3" s="7" t="s">
+        <v>18</v>
+      </c>
       <c r="HA3" s="6"/>
       <c r="AAA3" s="6"/>
     </row>
-    <row r="4" spans="1:703">
+    <row r="4" spans="1:703" ht="306">
+      <c r="A4" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="B4" s="7" t="s">
+        <v>19</v>
+      </c>
       <c r="HA4" s="4"/>
       <c r="AAA4" s="5"/>
     </row>
     <row r="5" spans="1:703">
+      <c r="A5" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="B5" s="2" t="s">
+        <v>21</v>
+      </c>
       <c r="HA5" s="4"/>
       <c r="AAA5" s="5"/>
     </row>
     <row r="6" spans="1:703">
+      <c r="A6" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="B6" s="2" t="s">
+        <v>23</v>
+      </c>
       <c r="HA6" s="4"/>
       <c r="AAA6" s="5"/>
     </row>

</xml_diff>